<commit_message>
chg: Updated tgt list with SYTGT058 and 061
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.3.xlsx
+++ b/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.3.xlsx
@@ -2944,11 +2944,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2961,6 +2956,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -2994,7 +2994,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3028,7 +3028,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3252,9 +3252,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B125" sqref="B125"/>
+      <selection pane="topRight" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3272,16 +3272,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="71" t="s">
@@ -3322,7 +3322,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="24">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="88" t="s">
         <v>617</v>
       </c>
       <c r="B4" s="84" t="s">
@@ -3346,7 +3346,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="89" t="s">
         <v>618</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -3370,7 +3370,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="90" t="s">
         <v>619</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -3394,7 +3394,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="89" t="s">
         <v>620</v>
       </c>
       <c r="B7" s="19" t="s">
@@ -3418,7 +3418,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="24">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="90" t="s">
         <v>621</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -3442,7 +3442,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="24">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="89" t="s">
         <v>622</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -3466,7 +3466,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="90" t="s">
         <v>623</v>
       </c>
       <c r="B10" s="24" t="s">
@@ -3490,7 +3490,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.25">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="89" t="s">
         <v>624</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -3514,7 +3514,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="90" t="s">
         <v>625</v>
       </c>
       <c r="B12" s="24" t="s">
@@ -3538,7 +3538,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.25">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="89" t="s">
         <v>626</v>
       </c>
       <c r="B13" s="26" t="s">
@@ -3562,7 +3562,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="90" t="s">
         <v>627</v>
       </c>
       <c r="B14" s="24" t="s">
@@ -3586,7 +3586,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.25">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="89" t="s">
         <v>628</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -3610,7 +3610,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.25">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="90" t="s">
         <v>629</v>
       </c>
       <c r="B16" s="24" t="s">
@@ -3634,7 +3634,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.25">
-      <c r="A17" s="92" t="s">
+      <c r="A17" s="89" t="s">
         <v>630</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -3658,7 +3658,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.25">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="90" t="s">
         <v>631</v>
       </c>
       <c r="B18" s="24" t="s">
@@ -3682,7 +3682,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.25">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="89" t="s">
         <v>632</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -3706,7 +3706,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="90" t="s">
         <v>633</v>
       </c>
       <c r="B20" s="24" t="s">
@@ -3730,7 +3730,7 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="92" t="s">
+      <c r="A21" s="89" t="s">
         <v>634</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -3757,7 +3757,7 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="24">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="90" t="s">
         <v>635</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -3781,7 +3781,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="24">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="89" t="s">
         <v>636</v>
       </c>
       <c r="B23" s="29" t="s">
@@ -3805,7 +3805,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.25">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="90" t="s">
         <v>637</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -3829,7 +3829,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="24">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="89" t="s">
         <v>638</v>
       </c>
       <c r="B25" s="22" t="s">
@@ -3853,7 +3853,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.25">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="90" t="s">
         <v>639</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -3877,7 +3877,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.25">
-      <c r="A27" s="92" t="s">
+      <c r="A27" s="89" t="s">
         <v>640</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -3901,7 +3901,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="93" t="s">
+      <c r="A28" s="90" t="s">
         <v>641</v>
       </c>
       <c r="B28" s="24" t="s">
@@ -3925,7 +3925,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="89" t="s">
         <v>642</v>
       </c>
       <c r="B29" s="26" t="s">
@@ -3949,7 +3949,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="90" t="s">
         <v>643</v>
       </c>
       <c r="B30" s="24" t="s">
@@ -4117,7 +4117,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="89" t="s">
         <v>650</v>
       </c>
       <c r="B37" s="22" t="s">
@@ -4141,7 +4141,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="90" t="s">
         <v>651</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -4237,7 +4237,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="90" t="s">
         <v>655</v>
       </c>
       <c r="B42" s="35" t="s">
@@ -4261,7 +4261,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A43" s="92" t="s">
+      <c r="A43" s="89" t="s">
         <v>656</v>
       </c>
       <c r="B43" s="22" t="s">
@@ -4285,7 +4285,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="90" t="s">
         <v>657</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -4567,7 +4567,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="93" t="s">
+      <c r="A56" s="90" t="s">
         <v>669</v>
       </c>
       <c r="B56" s="18" t="s">
@@ -4663,7 +4663,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="90" t="s">
         <v>673</v>
       </c>
       <c r="B60" s="15" t="s">
@@ -4687,7 +4687,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A61" s="58" t="s">
+      <c r="A61" s="89" t="s">
         <v>674</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -4711,7 +4711,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="25.5" customHeight="1">
-      <c r="A62" s="93" t="s">
+      <c r="A62" s="90" t="s">
         <v>675</v>
       </c>
       <c r="B62" s="15" t="s">
@@ -4735,7 +4735,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A63" s="92" t="s">
+      <c r="A63" s="89" t="s">
         <v>676</v>
       </c>
       <c r="B63" s="19" t="s">
@@ -4759,7 +4759,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="90" t="s">
         <v>677</v>
       </c>
       <c r="B64" s="15" t="s">
@@ -4879,7 +4879,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="89" t="s">
         <v>682</v>
       </c>
       <c r="B69" s="22" t="s">
@@ -4903,7 +4903,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A70" s="93" t="s">
+      <c r="A70" s="90" t="s">
         <v>683</v>
       </c>
       <c r="B70" s="18" t="s">
@@ -4927,7 +4927,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A71" s="92" t="s">
+      <c r="A71" s="89" t="s">
         <v>684</v>
       </c>
       <c r="B71" s="22" t="s">
@@ -4951,7 +4951,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="25.5" customHeight="1">
-      <c r="A72" s="93" t="s">
+      <c r="A72" s="90" t="s">
         <v>685</v>
       </c>
       <c r="B72" s="18" t="s">
@@ -4975,7 +4975,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="28.5" customHeight="1">
-      <c r="A73" s="92" t="s">
+      <c r="A73" s="89" t="s">
         <v>686</v>
       </c>
       <c r="B73" s="22" t="s">
@@ -5023,7 +5023,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A75" s="92" t="s">
+      <c r="A75" s="89" t="s">
         <v>688</v>
       </c>
       <c r="B75" s="22" t="s">
@@ -5047,7 +5047,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A76" s="93" t="s">
+      <c r="A76" s="90" t="s">
         <v>689</v>
       </c>
       <c r="B76" s="18" t="s">
@@ -5071,7 +5071,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A77" s="92" t="s">
+      <c r="A77" s="89" t="s">
         <v>690</v>
       </c>
       <c r="B77" s="22" t="s">
@@ -5095,7 +5095,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A78" s="93" t="s">
+      <c r="A78" s="90" t="s">
         <v>691</v>
       </c>
       <c r="B78" s="18" t="s">
@@ -5359,7 +5359,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A89" s="92" t="s">
+      <c r="A89" s="89" t="s">
         <v>702</v>
       </c>
       <c r="B89" s="22" t="s">
@@ -5407,7 +5407,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A91" s="92" t="s">
+      <c r="A91" s="89" t="s">
         <v>704</v>
       </c>
       <c r="B91" s="22" t="s">
@@ -5431,7 +5431,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="45.75" customHeight="1">
-      <c r="A92" s="93" t="s">
+      <c r="A92" s="90" t="s">
         <v>705</v>
       </c>
       <c r="B92" s="18" t="s">
@@ -5479,7 +5479,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A94" s="93" t="s">
+      <c r="A94" s="90" t="s">
         <v>707</v>
       </c>
       <c r="B94" s="15" t="s">
@@ -5551,7 +5551,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A97" s="92" t="s">
+      <c r="A97" s="89" t="s">
         <v>710</v>
       </c>
       <c r="B97" s="22" t="s">
@@ -5647,7 +5647,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="24">
-      <c r="A101" s="92" t="s">
+      <c r="A101" s="89" t="s">
         <v>714</v>
       </c>
       <c r="B101" s="22" t="s">
@@ -5767,7 +5767,7 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A106" s="93" t="s">
+      <c r="A106" s="90" t="s">
         <v>719</v>
       </c>
       <c r="B106" s="18" t="s">
@@ -6449,7 +6449,7 @@
       <c r="H137" s="65"/>
     </row>
     <row r="138" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A138" s="94" t="s">
+      <c r="A138" s="91" t="s">
         <v>751</v>
       </c>
       <c r="B138" s="66" t="s">
@@ -12848,9 +12848,11 @@
     <hyperlink ref="A78" r:id="rId51"/>
     <hyperlink ref="A94" r:id="rId52"/>
     <hyperlink ref="A138" r:id="rId53"/>
+    <hyperlink ref="A61" r:id="rId54"/>
+    <hyperlink ref="A64" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId54"/>
-  <drawing r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId56"/>
+  <drawing r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>